<commit_message>
exported clean data to new excel file
</commit_message>
<xml_diff>
--- a/Fitabase and Consent Dates File 2.1.23.xlsx
+++ b/Fitabase and Consent Dates File 2.1.23.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tylerwong/Documents/workspace/research lab/happy_teacher/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tyler.wong\Desktop\happy_teacher\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B6DC10-DB74-8F41-A476-DD3FB27F853D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{2EA3ABA9-E61D-4CF2-8EAE-9E3B2D751FDF}"/>
+    <workbookView xWindow="-38400" yWindow="495" windowWidth="38400" windowHeight="21105"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$1</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="148">
   <si>
     <t>ID</t>
   </si>
@@ -228,14 +227,269 @@
   </si>
   <si>
     <t>10804   2022-11-01</t>
+  </si>
+  <si>
+    <t>starting -&gt; first data point</t>
+  </si>
+  <si>
+    <t># of days of intervention</t>
+  </si>
+  <si>
+    <t>10101   2022-10-27</t>
+  </si>
+  <si>
+    <t>10102   2022-12-09</t>
+  </si>
+  <si>
+    <t>10103   2022-12-21</t>
+  </si>
+  <si>
+    <t>10104   2022-11-03</t>
+  </si>
+  <si>
+    <t>10106   2022-10-19</t>
+  </si>
+  <si>
+    <t>10107   2022-12-07</t>
+  </si>
+  <si>
+    <t>10108   2022-11-22</t>
+  </si>
+  <si>
+    <t>10109   2022-11-20</t>
+  </si>
+  <si>
+    <t>10204   2022-12-13</t>
+  </si>
+  <si>
+    <t>10205   2022-12-07</t>
+  </si>
+  <si>
+    <t>10301   2022-12-22</t>
+  </si>
+  <si>
+    <t>10302   2022-11-12</t>
+  </si>
+  <si>
+    <t>10303   2022-11-21</t>
+  </si>
+  <si>
+    <t>10304   2022-12-31</t>
+  </si>
+  <si>
+    <t>10305   2022-12-19</t>
+  </si>
+  <si>
+    <t>10306   2022-12-05</t>
+  </si>
+  <si>
+    <t>10307   2022-12-31</t>
+  </si>
+  <si>
+    <t>10401   2022-12-01</t>
+  </si>
+  <si>
+    <t>10402   2022-12-14</t>
+  </si>
+  <si>
+    <t>10403   2022-12-02</t>
+  </si>
+  <si>
+    <t>10404   2022-12-10</t>
+  </si>
+  <si>
+    <t>10405   2022-12-07</t>
+  </si>
+  <si>
+    <t>10406   2022-12-31</t>
+  </si>
+  <si>
+    <t>10407   2022-12-31</t>
+  </si>
+  <si>
+    <t>10408   2022-12-16</t>
+  </si>
+  <si>
+    <t>10409   2022-12-14</t>
+  </si>
+  <si>
+    <t>10410   2022-12-31</t>
+  </si>
+  <si>
+    <t>10412   2022-11-17</t>
+  </si>
+  <si>
+    <t>10413   2022-12-06</t>
+  </si>
+  <si>
+    <t>10501   2022-12-10</t>
+  </si>
+  <si>
+    <t>10502   2022-12-13</t>
+  </si>
+  <si>
+    <t>10503   2022-12-17</t>
+  </si>
+  <si>
+    <t>10504   2022-12-19</t>
+  </si>
+  <si>
+    <t>10505   2022-12-19</t>
+  </si>
+  <si>
+    <t>10601   2022-11-27</t>
+  </si>
+  <si>
+    <t>10602   2022-12-31</t>
+  </si>
+  <si>
+    <t>10603   2022-12-15</t>
+  </si>
+  <si>
+    <t>10604   2022-12-29</t>
+  </si>
+  <si>
+    <t>10605   2022-12-06</t>
+  </si>
+  <si>
+    <t>10606   2022-10-29</t>
+  </si>
+  <si>
+    <t>10607   2022-12-07</t>
+  </si>
+  <si>
+    <t>10608   2022-11-16</t>
+  </si>
+  <si>
+    <t>10609   2022-11-17</t>
+  </si>
+  <si>
+    <t>10610   2022-12-19</t>
+  </si>
+  <si>
+    <t>10611   2022-12-09</t>
+  </si>
+  <si>
+    <t>10612   2022-12-13</t>
+  </si>
+  <si>
+    <t>10613   2022-11-09</t>
+  </si>
+  <si>
+    <t>10614   2022-11-05</t>
+  </si>
+  <si>
+    <t>10615   2022-12-09</t>
+  </si>
+  <si>
+    <t>10616   2022-11-27</t>
+  </si>
+  <si>
+    <t>10701   2023-01-08</t>
+  </si>
+  <si>
+    <t>10702   2022-12-20</t>
+  </si>
+  <si>
+    <t>10703   2023-01-03</t>
+  </si>
+  <si>
+    <t>10704   2022-12-27</t>
+  </si>
+  <si>
+    <t>10801   2023-01-17</t>
+  </si>
+  <si>
+    <t>10802   2022-12-14</t>
+  </si>
+  <si>
+    <t>10803   2022-12-05</t>
+  </si>
+  <si>
+    <t>10804   2022-12-12</t>
+  </si>
+  <si>
+    <t>10104   2022-10-18</t>
+  </si>
+  <si>
+    <t>10106   2022-10-18</t>
+  </si>
+  <si>
+    <t>10109   2022-11-19</t>
+  </si>
+  <si>
+    <t>10205   2022-12-06</t>
+  </si>
+  <si>
+    <t>10301   2022-12-21</t>
+  </si>
+  <si>
+    <t>10303   2022-11-18</t>
+  </si>
+  <si>
+    <t>10305   2022-12-18</t>
+  </si>
+  <si>
+    <t>10408   2022-12-15</t>
+  </si>
+  <si>
+    <t>10409   2022-12-13</t>
+  </si>
+  <si>
+    <t>10412   2022-11-16</t>
+  </si>
+  <si>
+    <t>10413   2022-12-05</t>
+  </si>
+  <si>
+    <t>10415   2023-01-15</t>
+  </si>
+  <si>
+    <t>10501   2022-12-09</t>
+  </si>
+  <si>
+    <t>10502   2022-12-12</t>
+  </si>
+  <si>
+    <t>10505   2022-12-18</t>
+  </si>
+  <si>
+    <t>10601   2022-11-25</t>
+  </si>
+  <si>
+    <t>10605   2022-11-22</t>
+  </si>
+  <si>
+    <t>10607   2022-12-06</t>
+  </si>
+  <si>
+    <t>10608   2022-11-13</t>
+  </si>
+  <si>
+    <t>10610   2022-12-15</t>
+  </si>
+  <si>
+    <t>10614   2022-11-04</t>
+  </si>
+  <si>
+    <t>10616   2022-11-24</t>
+  </si>
+  <si>
+    <t>10701   2022-12-24</t>
+  </si>
+  <si>
+    <t>10703   2023-01-02</t>
+  </si>
+  <si>
+    <t>10802   2022-12-04</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -249,11 +503,13 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -350,15 +606,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="3" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_Sheet1" xfId="1" xr:uid="{109761DA-583C-40EB-BEE5-FCEB8066D124}"/>
+    <cellStyle name="Normal_Sheet1" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -669,23 +925,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96BA85B1-AB98-4316-911B-E527142C00CD}">
-  <dimension ref="A1:L60"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V16" sqref="V16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" customWidth="1"/>
-    <col min="5" max="5" width="12.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="7"/>
+    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="7"/>
+    <col min="10" max="10" width="11.42578125" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" customWidth="1"/>
+    <col min="20" max="20" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -702,60 +961,121 @@
         <v>4</v>
       </c>
       <c r="G1" s="6"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L1" t="s">
+        <v>63</v>
+      </c>
+      <c r="U1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>10415</v>
+        <v>10101</v>
       </c>
       <c r="B2" s="2" t="b">
         <v>1</v>
       </c>
       <c r="C2" s="3">
-        <v>44860</v>
+        <v>44830</v>
       </c>
       <c r="D2" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E2" s="3">
-        <v>44860</v>
+        <v>44854</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="J2" s="5">
-        <v>44860</v>
+        <v>44839</v>
+      </c>
+      <c r="K2" s="5">
+        <f>J2</f>
+        <v>44839</v>
       </c>
       <c r="L2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+        <f>J2-C2</f>
+        <v>9</v>
+      </c>
+      <c r="M2" t="str">
+        <f>M31&amp;","&amp;L2</f>
+        <v>0,9</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="O2" s="7"/>
+      <c r="Q2" t="s">
+        <v>65</v>
+      </c>
+      <c r="T2" s="5">
+        <v>44861</v>
+      </c>
+      <c r="V2">
+        <f>T2-C2</f>
+        <v>31</v>
+      </c>
+      <c r="W2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>10101</v>
+        <v>10102</v>
       </c>
       <c r="B3" s="2" t="b">
         <v>1</v>
       </c>
       <c r="C3" s="3">
-        <v>44830</v>
+        <v>44834</v>
       </c>
       <c r="D3" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E3" s="3">
-        <v>44854</v>
+        <v>44840</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="J3" s="5">
         <v>44839</v>
       </c>
+      <c r="K3" t="str">
+        <f>K2&amp;","&amp;J3</f>
+        <v>44839,44839</v>
+      </c>
       <c r="L3">
-        <f>J3-C3</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+        <f t="shared" ref="L3:L60" si="0">J3-C3</f>
+        <v>5</v>
+      </c>
+      <c r="M3" t="str">
+        <f t="shared" ref="M3:M60" si="1">M2&amp;","&amp;L3</f>
+        <v>0,9,5</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="O3" s="7"/>
+      <c r="Q3" t="s">
+        <v>66</v>
+      </c>
+      <c r="T3" s="5">
+        <v>44904</v>
+      </c>
+      <c r="V3">
+        <f>T3-C3</f>
+        <v>70</v>
+      </c>
+      <c r="W3" t="str">
+        <f t="shared" ref="W3:W60" si="2">W2&amp;","&amp;V3</f>
+        <v>31,70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>10102</v>
+        <v>10103</v>
       </c>
       <c r="B4" s="2" t="b">
         <v>1</v>
@@ -767,22 +1087,48 @@
         <v>1</v>
       </c>
       <c r="E4" s="3">
-        <v>44840</v>
+        <v>44845</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J4" s="5">
         <v>44839</v>
       </c>
+      <c r="K4" t="str">
+        <f t="shared" ref="K4:K6" si="3">K3&amp;","&amp;J4</f>
+        <v>44839,44839,44839</v>
+      </c>
       <c r="L4">
-        <f t="shared" ref="L4:L60" si="0">J4-C4</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M4" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="O4" s="7"/>
+      <c r="Q4" t="s">
+        <v>67</v>
+      </c>
+      <c r="T4" s="5">
+        <v>44916</v>
+      </c>
+      <c r="V4">
+        <f>T4-C4</f>
+        <v>82</v>
+      </c>
+      <c r="W4" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>10103</v>
+        <v>10104</v>
       </c>
       <c r="B5" s="2" t="b">
         <v>1</v>
@@ -794,22 +1140,48 @@
         <v>1</v>
       </c>
       <c r="E5" s="3">
-        <v>44845</v>
+        <v>44854</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J5" s="5">
         <v>44839</v>
       </c>
+      <c r="K5" t="str">
+        <f t="shared" si="3"/>
+        <v>44839,44839,44839,44839</v>
+      </c>
       <c r="L5">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M5" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="O5" s="7"/>
+      <c r="Q5" t="s">
+        <v>123</v>
+      </c>
+      <c r="T5" s="5">
+        <v>44852</v>
+      </c>
+      <c r="V5">
+        <f>T5-C5</f>
+        <v>18</v>
+      </c>
+      <c r="W5" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>10104</v>
+        <v>10106</v>
       </c>
       <c r="B6" s="2" t="b">
         <v>1</v>
@@ -821,22 +1193,48 @@
         <v>1</v>
       </c>
       <c r="E6" s="3">
-        <v>44854</v>
+        <v>44840</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J6" s="5">
         <v>44839</v>
       </c>
+      <c r="K6" t="str">
+        <f t="shared" si="3"/>
+        <v>44839,44839,44839,44839,44839</v>
+      </c>
       <c r="L6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M6" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="O6" s="7"/>
+      <c r="Q6" t="s">
+        <v>124</v>
+      </c>
+      <c r="T6" s="5">
+        <v>44852</v>
+      </c>
+      <c r="V6">
+        <f>T6-C6</f>
+        <v>18</v>
+      </c>
+      <c r="W6" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>10106</v>
+        <v>10107</v>
       </c>
       <c r="B7" s="2" t="b">
         <v>1</v>
@@ -848,10 +1246,10 @@
         <v>1</v>
       </c>
       <c r="E7" s="3">
-        <v>44840</v>
+        <v>44841</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J7" s="5">
         <v>44839</v>
@@ -860,10 +1258,32 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M7" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="O7" s="7"/>
+      <c r="Q7" t="s">
+        <v>70</v>
+      </c>
+      <c r="T7" s="5">
+        <v>44902</v>
+      </c>
+      <c r="V7">
+        <f>T7-C7</f>
+        <v>68</v>
+      </c>
+      <c r="W7" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>10107</v>
+        <v>10108</v>
       </c>
       <c r="B8" s="2" t="b">
         <v>1</v>
@@ -875,10 +1295,10 @@
         <v>1</v>
       </c>
       <c r="E8" s="3">
-        <v>44841</v>
+        <v>44840</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J8" s="5">
         <v>44839</v>
@@ -887,10 +1307,32 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M8" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5</v>
+      </c>
+      <c r="N8" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="O8" s="7"/>
+      <c r="Q8" t="s">
+        <v>71</v>
+      </c>
+      <c r="T8" s="5">
+        <v>44887</v>
+      </c>
+      <c r="V8">
+        <f>T8-C8</f>
+        <v>53</v>
+      </c>
+      <c r="W8" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>10108</v>
+        <v>10109</v>
       </c>
       <c r="B9" s="2" t="b">
         <v>1</v>
@@ -902,10 +1344,10 @@
         <v>1</v>
       </c>
       <c r="E9" s="3">
-        <v>44840</v>
+        <v>44841</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J9" s="5">
         <v>44839</v>
@@ -914,37 +1356,81 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M9" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5</v>
+      </c>
+      <c r="N9" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="O9" s="7"/>
+      <c r="Q9" t="s">
+        <v>125</v>
+      </c>
+      <c r="T9" s="5">
+        <v>44884</v>
+      </c>
+      <c r="V9">
+        <f>T9-C9</f>
+        <v>50</v>
+      </c>
+      <c r="W9" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>10109</v>
+        <v>10204</v>
       </c>
       <c r="B10" s="2" t="b">
         <v>1</v>
       </c>
       <c r="C10" s="3">
-        <v>44834</v>
+        <v>44837</v>
       </c>
       <c r="D10" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E10" s="3">
-        <v>44841</v>
+        <v>44839</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J10" s="5">
         <v>44839</v>
       </c>
       <c r="L10">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="M10" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2</v>
+      </c>
+      <c r="N10" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="O10" s="7"/>
+      <c r="Q10" t="s">
+        <v>73</v>
+      </c>
+      <c r="T10" s="5">
+        <v>44908</v>
+      </c>
+      <c r="V10">
+        <f>T10-C10</f>
+        <v>71</v>
+      </c>
+      <c r="W10" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>10204</v>
+        <v>10205</v>
       </c>
       <c r="B11" s="2" t="b">
         <v>1</v>
@@ -956,10 +1442,10 @@
         <v>1</v>
       </c>
       <c r="E11" s="3">
-        <v>44839</v>
+        <v>44844</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J11" s="5">
         <v>44839</v>
@@ -968,37 +1454,81 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M11" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2</v>
+      </c>
+      <c r="N11" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="O11" s="7"/>
+      <c r="Q11" t="s">
+        <v>126</v>
+      </c>
+      <c r="T11" s="5">
+        <v>44901</v>
+      </c>
+      <c r="V11">
+        <f>T11-C11</f>
+        <v>64</v>
+      </c>
+      <c r="W11" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>10205</v>
+        <v>10301</v>
       </c>
       <c r="B12" s="2" t="b">
         <v>1</v>
       </c>
       <c r="C12" s="3">
-        <v>44837</v>
+        <v>44838</v>
       </c>
       <c r="D12" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E12" s="3">
-        <v>44844</v>
+        <v>44845</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J12" s="5">
-        <v>44839</v>
+        <v>44861</v>
       </c>
       <c r="L12">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="M12" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23</v>
+      </c>
+      <c r="N12" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="O12" s="7"/>
+      <c r="Q12" t="s">
+        <v>127</v>
+      </c>
+      <c r="T12" s="5">
+        <v>44916</v>
+      </c>
+      <c r="V12">
+        <f>T12-C12</f>
+        <v>78</v>
+      </c>
+      <c r="W12" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>10301</v>
+        <v>10302</v>
       </c>
       <c r="B13" s="2" t="b">
         <v>1</v>
@@ -1010,22 +1540,44 @@
         <v>1</v>
       </c>
       <c r="E13" s="3">
-        <v>44845</v>
+        <v>44840</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J13" s="5">
-        <v>44861</v>
+        <v>44839</v>
       </c>
       <c r="L13">
         <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="M13" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1</v>
+      </c>
+      <c r="N13" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="O13" s="7"/>
+      <c r="Q13" t="s">
+        <v>76</v>
+      </c>
+      <c r="T13" s="5">
+        <v>44877</v>
+      </c>
+      <c r="V13">
+        <f>T13-C13</f>
+        <v>39</v>
+      </c>
+      <c r="W13" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>10302</v>
+        <v>10303</v>
       </c>
       <c r="B14" s="2" t="b">
         <v>1</v>
@@ -1037,10 +1589,10 @@
         <v>1</v>
       </c>
       <c r="E14" s="3">
-        <v>44840</v>
+        <v>44847</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J14" s="5">
         <v>44839</v>
@@ -1049,10 +1601,32 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M14" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1,1</v>
+      </c>
+      <c r="N14" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="O14" s="7"/>
+      <c r="Q14" t="s">
+        <v>128</v>
+      </c>
+      <c r="T14" s="5">
+        <v>44883</v>
+      </c>
+      <c r="V14">
+        <f>T14-C14</f>
+        <v>45</v>
+      </c>
+      <c r="W14" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>10303</v>
+        <v>10304</v>
       </c>
       <c r="B15" s="2" t="b">
         <v>1</v>
@@ -1064,10 +1638,10 @@
         <v>1</v>
       </c>
       <c r="E15" s="3">
-        <v>44847</v>
+        <v>44861</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J15" s="5">
         <v>44839</v>
@@ -1076,10 +1650,32 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M15" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1,1,1</v>
+      </c>
+      <c r="N15" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="O15" s="7"/>
+      <c r="Q15" t="s">
+        <v>78</v>
+      </c>
+      <c r="T15" s="5">
+        <v>44926</v>
+      </c>
+      <c r="V15">
+        <f>T15-C15</f>
+        <v>88</v>
+      </c>
+      <c r="W15" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45,88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>10304</v>
+        <v>10305</v>
       </c>
       <c r="B16" s="2" t="b">
         <v>1</v>
@@ -1091,22 +1687,44 @@
         <v>1</v>
       </c>
       <c r="E16" s="3">
-        <v>44861</v>
+        <v>44852</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J16" s="5">
-        <v>44839</v>
+        <v>44852</v>
       </c>
       <c r="L16">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="M16" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1,1,1,14</v>
+      </c>
+      <c r="N16" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="O16" s="7"/>
+      <c r="Q16" t="s">
+        <v>129</v>
+      </c>
+      <c r="T16" s="5">
+        <v>44913</v>
+      </c>
+      <c r="V16">
+        <f>T16-C16</f>
+        <v>75</v>
+      </c>
+      <c r="W16" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45,88,75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>10305</v>
+        <v>10306</v>
       </c>
       <c r="B17" s="2" t="b">
         <v>1</v>
@@ -1118,22 +1736,44 @@
         <v>1</v>
       </c>
       <c r="E17" s="3">
-        <v>44852</v>
+        <v>44840</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="J17" s="5">
-        <v>44852</v>
+        <v>19</v>
+      </c>
+      <c r="J17" s="8">
+        <v>44839</v>
       </c>
       <c r="L17">
         <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="M17" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1,1,1,14,1</v>
+      </c>
+      <c r="N17" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="O17" s="7"/>
+      <c r="Q17" t="s">
+        <v>80</v>
+      </c>
+      <c r="T17" s="5">
+        <v>44900</v>
+      </c>
+      <c r="V17">
+        <f>T17-C17</f>
+        <v>62</v>
+      </c>
+      <c r="W17" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45,88,75,62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>10306</v>
+        <v>10307</v>
       </c>
       <c r="B18" s="2" t="b">
         <v>1</v>
@@ -1145,10 +1785,10 @@
         <v>1</v>
       </c>
       <c r="E18" s="3">
-        <v>44840</v>
+        <v>44845</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J18" s="8">
         <v>44839</v>
@@ -1157,37 +1797,81 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M18" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1,1,1,14,1,1</v>
+      </c>
+      <c r="N18" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="O18" s="7"/>
+      <c r="Q18" t="s">
+        <v>81</v>
+      </c>
+      <c r="T18" s="5">
+        <v>44926</v>
+      </c>
+      <c r="V18">
+        <f>T18-C18</f>
+        <v>88</v>
+      </c>
+      <c r="W18" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45,88,75,62,88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>10307</v>
+        <v>10401</v>
       </c>
       <c r="B19" s="2" t="b">
         <v>1</v>
       </c>
       <c r="C19" s="3">
-        <v>44838</v>
+        <v>44845</v>
       </c>
       <c r="D19" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E19" s="3">
-        <v>44845</v>
+        <v>44859</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="J19" s="8">
-        <v>44839</v>
+        <v>21</v>
+      </c>
+      <c r="J19" s="5">
+        <v>44855</v>
       </c>
       <c r="L19">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="M19" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1,1,1,14,1,1,10</v>
+      </c>
+      <c r="N19" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="O19" s="7"/>
+      <c r="Q19" t="s">
+        <v>82</v>
+      </c>
+      <c r="T19" s="5">
+        <v>44896</v>
+      </c>
+      <c r="V19">
+        <f>T19-C19</f>
+        <v>51</v>
+      </c>
+      <c r="W19" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45,88,75,62,88,51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>10401</v>
+        <v>10402</v>
       </c>
       <c r="B20" s="2" t="b">
         <v>1</v>
@@ -1199,22 +1883,44 @@
         <v>1</v>
       </c>
       <c r="E20" s="3">
-        <v>44859</v>
+        <v>44851</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J20" s="5">
-        <v>44855</v>
+        <v>44847</v>
       </c>
       <c r="L20">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="M20" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1,1,1,14,1,1,10,2</v>
+      </c>
+      <c r="N20" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="O20" s="7"/>
+      <c r="Q20" t="s">
+        <v>83</v>
+      </c>
+      <c r="T20" s="5">
+        <v>44909</v>
+      </c>
+      <c r="V20">
+        <f>T20-C20</f>
+        <v>64</v>
+      </c>
+      <c r="W20" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45,88,75,62,88,51,64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>10402</v>
+        <v>10403</v>
       </c>
       <c r="B21" s="2" t="b">
         <v>1</v>
@@ -1226,22 +1932,44 @@
         <v>1</v>
       </c>
       <c r="E21" s="3">
-        <v>44851</v>
+        <v>44859</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J21" s="5">
-        <v>44847</v>
+        <v>44846</v>
       </c>
       <c r="L21">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="M21" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1,1,1,14,1,1,10,2,1</v>
+      </c>
+      <c r="N21" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="O21" s="7"/>
+      <c r="Q21" t="s">
+        <v>84</v>
+      </c>
+      <c r="T21" s="5">
+        <v>44897</v>
+      </c>
+      <c r="V21">
+        <f>T21-C21</f>
+        <v>52</v>
+      </c>
+      <c r="W21" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45,88,75,62,88,51,64,52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>10403</v>
+        <v>10404</v>
       </c>
       <c r="B22" s="2" t="b">
         <v>1</v>
@@ -1253,10 +1981,10 @@
         <v>1</v>
       </c>
       <c r="E22" s="3">
-        <v>44859</v>
+        <v>44847</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J22" s="5">
         <v>44846</v>
@@ -1265,10 +1993,32 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M22" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1,1,1,14,1,1,10,2,1,1</v>
+      </c>
+      <c r="N22" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="O22" s="7"/>
+      <c r="Q22" t="s">
+        <v>85</v>
+      </c>
+      <c r="T22" s="5">
+        <v>44905</v>
+      </c>
+      <c r="V22">
+        <f>T22-C22</f>
+        <v>60</v>
+      </c>
+      <c r="W22" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45,88,75,62,88,51,64,52,60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>10404</v>
+        <v>10405</v>
       </c>
       <c r="B23" s="2" t="b">
         <v>1</v>
@@ -1280,10 +2030,10 @@
         <v>1</v>
       </c>
       <c r="E23" s="3">
-        <v>44847</v>
+        <v>44851</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J23" s="5">
         <v>44846</v>
@@ -1292,10 +2042,32 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M23" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1,1,1,14,1,1,10,2,1,1,1</v>
+      </c>
+      <c r="N23" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="O23" s="7"/>
+      <c r="Q23" t="s">
+        <v>86</v>
+      </c>
+      <c r="T23" s="5">
+        <v>44902</v>
+      </c>
+      <c r="V23">
+        <f>T23-C23</f>
+        <v>57</v>
+      </c>
+      <c r="W23" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45,88,75,62,88,51,64,52,60,57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>10405</v>
+        <v>10406</v>
       </c>
       <c r="B24" s="2" t="b">
         <v>1</v>
@@ -1307,10 +2079,10 @@
         <v>1</v>
       </c>
       <c r="E24" s="3">
-        <v>44851</v>
+        <v>44846</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J24" s="5">
         <v>44846</v>
@@ -1319,10 +2091,32 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M24" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1,1,1,14,1,1,10,2,1,1,1,1</v>
+      </c>
+      <c r="N24" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="O24" s="7"/>
+      <c r="Q24" t="s">
+        <v>87</v>
+      </c>
+      <c r="T24" s="5">
+        <v>44926</v>
+      </c>
+      <c r="V24">
+        <f>T24-C24</f>
+        <v>81</v>
+      </c>
+      <c r="W24" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45,88,75,62,88,51,64,52,60,57,81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>10406</v>
+        <v>10407</v>
       </c>
       <c r="B25" s="2" t="b">
         <v>1</v>
@@ -1334,10 +2128,10 @@
         <v>1</v>
       </c>
       <c r="E25" s="3">
-        <v>44846</v>
+        <v>44847</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J25" s="5">
         <v>44846</v>
@@ -1346,10 +2140,32 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M25" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1,1,1,14,1,1,10,2,1,1,1,1,1</v>
+      </c>
+      <c r="N25" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="O25" s="7"/>
+      <c r="Q25" t="s">
+        <v>88</v>
+      </c>
+      <c r="T25" s="5">
+        <v>44926</v>
+      </c>
+      <c r="V25">
+        <f>T25-C25</f>
+        <v>81</v>
+      </c>
+      <c r="W25" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45,88,75,62,88,51,64,52,60,57,81,81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>10407</v>
+        <v>10408</v>
       </c>
       <c r="B26" s="2" t="b">
         <v>1</v>
@@ -1361,10 +2177,10 @@
         <v>1</v>
       </c>
       <c r="E26" s="3">
-        <v>44847</v>
+        <v>44854</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J26" s="5">
         <v>44846</v>
@@ -1373,10 +2189,32 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M26" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1,1,1,14,1,1,10,2,1,1,1,1,1,1</v>
+      </c>
+      <c r="N26" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="O26" s="7"/>
+      <c r="Q26" t="s">
+        <v>130</v>
+      </c>
+      <c r="T26" s="5">
+        <v>44910</v>
+      </c>
+      <c r="V26">
+        <f>T26-C26</f>
+        <v>65</v>
+      </c>
+      <c r="W26" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45,88,75,62,88,51,64,52,60,57,81,81,65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>10408</v>
+        <v>10409</v>
       </c>
       <c r="B27" s="2" t="b">
         <v>1</v>
@@ -1388,10 +2226,10 @@
         <v>1</v>
       </c>
       <c r="E27" s="3">
-        <v>44854</v>
+        <v>44859</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J27" s="5">
         <v>44846</v>
@@ -1400,10 +2238,32 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M27" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1,1,1,14,1,1,10,2,1,1,1,1,1,1,1</v>
+      </c>
+      <c r="N27" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="O27" s="7"/>
+      <c r="Q27" t="s">
+        <v>131</v>
+      </c>
+      <c r="T27" s="5">
+        <v>44908</v>
+      </c>
+      <c r="V27">
+        <f>T27-C27</f>
+        <v>63</v>
+      </c>
+      <c r="W27" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45,88,75,62,88,51,64,52,60,57,81,81,65,63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>10409</v>
+        <v>10410</v>
       </c>
       <c r="B28" s="2" t="b">
         <v>1</v>
@@ -1415,10 +2275,10 @@
         <v>1</v>
       </c>
       <c r="E28" s="3">
-        <v>44859</v>
+        <v>44847</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J28" s="5">
         <v>44846</v>
@@ -1427,10 +2287,32 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M28" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1,1,1,14,1,1,10,2,1,1,1,1,1,1,1,1</v>
+      </c>
+      <c r="N28" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="O28" s="7"/>
+      <c r="Q28" t="s">
+        <v>91</v>
+      </c>
+      <c r="T28" s="5">
+        <v>44926</v>
+      </c>
+      <c r="V28">
+        <f>T28-C28</f>
+        <v>81</v>
+      </c>
+      <c r="W28" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45,88,75,62,88,51,64,52,60,57,81,81,65,63,81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>10410</v>
+        <v>10412</v>
       </c>
       <c r="B29" s="2" t="b">
         <v>1</v>
@@ -1442,22 +2324,44 @@
         <v>1</v>
       </c>
       <c r="E29" s="3">
-        <v>44847</v>
+        <v>44860</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J29" s="5">
-        <v>44846</v>
+        <v>44860</v>
       </c>
       <c r="L29">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="M29" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1,1,1,14,1,1,10,2,1,1,1,1,1,1,1,1,15</v>
+      </c>
+      <c r="N29" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="O29" s="7"/>
+      <c r="Q29" t="s">
+        <v>132</v>
+      </c>
+      <c r="T29" s="5">
+        <v>44881</v>
+      </c>
+      <c r="V29">
+        <f>T29-C29</f>
+        <v>36</v>
+      </c>
+      <c r="W29" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45,88,75,62,88,51,64,52,60,57,81,81,65,63,81,36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>10412</v>
+        <v>10413</v>
       </c>
       <c r="B30" s="2" t="b">
         <v>1</v>
@@ -1469,47 +2373,82 @@
         <v>1</v>
       </c>
       <c r="E30" s="3">
+        <v>44859</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J30" s="5">
+        <v>44847</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="M30" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1,1,1,14,1,1,10,2,1,1,1,1,1,1,1,1,15,2</v>
+      </c>
+      <c r="N30" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="O30" s="7"/>
+      <c r="Q30" t="s">
+        <v>133</v>
+      </c>
+      <c r="T30" s="5">
+        <v>44900</v>
+      </c>
+      <c r="V30">
+        <f>T30-C30</f>
+        <v>55</v>
+      </c>
+      <c r="W30" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45,88,75,62,88,51,64,52,60,57,81,81,65,63,81,36,55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>10415</v>
+      </c>
+      <c r="B31" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3">
         <v>44860</v>
       </c>
-      <c r="G30" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="J30" s="5">
+      <c r="D31" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E31" s="3">
         <v>44860</v>
       </c>
-      <c r="L30">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="2">
-        <v>10413</v>
-      </c>
-      <c r="B31" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="C31" s="3">
-        <v>44845</v>
-      </c>
-      <c r="D31" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E31" s="3">
-        <v>44859</v>
-      </c>
-      <c r="G31" s="7" t="s">
-        <v>32</v>
-      </c>
       <c r="J31" s="5">
-        <v>44847</v>
+        <v>44860</v>
       </c>
       <c r="L31">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <v>0</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>134</v>
+      </c>
+      <c r="T31" s="5">
+        <v>44941</v>
+      </c>
+      <c r="V31">
+        <f>T31-C31</f>
+        <v>81</v>
+      </c>
+      <c r="W31" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45,88,75,62,88,51,64,52,60,57,81,81,65,63,81,36,55,81</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>10501</v>
       </c>
@@ -1535,8 +2474,29 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M32" t="str">
+        <f>M30&amp;","&amp;L32</f>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1,1,1,14,1,1,10,2,1,1,1,1,1,1,1,1,15,2,0</v>
+      </c>
+      <c r="N32" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>135</v>
+      </c>
+      <c r="T32" s="5">
+        <v>44904</v>
+      </c>
+      <c r="V32">
+        <f>T32-C32</f>
+        <v>57</v>
+      </c>
+      <c r="W32" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45,88,75,62,88,51,64,52,60,57,81,81,65,63,81,36,55,81,57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>10502</v>
       </c>
@@ -1562,8 +2522,29 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M33" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1,1,1,14,1,1,10,2,1,1,1,1,1,1,1,1,15,2,0,0</v>
+      </c>
+      <c r="N33" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>136</v>
+      </c>
+      <c r="T33" s="5">
+        <v>44907</v>
+      </c>
+      <c r="V33">
+        <f>T33-C33</f>
+        <v>60</v>
+      </c>
+      <c r="W33" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45,88,75,62,88,51,64,52,60,57,81,81,65,63,81,36,55,81,57,60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>10503</v>
       </c>
@@ -1589,8 +2570,29 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M34" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1,1,1,14,1,1,10,2,1,1,1,1,1,1,1,1,15,2,0,0,0</v>
+      </c>
+      <c r="N34" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>96</v>
+      </c>
+      <c r="T34" s="5">
+        <v>44912</v>
+      </c>
+      <c r="V34">
+        <f>T34-C34</f>
+        <v>65</v>
+      </c>
+      <c r="W34" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45,88,75,62,88,51,64,52,60,57,81,81,65,63,81,36,55,81,57,60,65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>10504</v>
       </c>
@@ -1616,8 +2618,29 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M35" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1,1,1,14,1,1,10,2,1,1,1,1,1,1,1,1,15,2,0,0,0,0</v>
+      </c>
+      <c r="N35" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>97</v>
+      </c>
+      <c r="T35" s="5">
+        <v>44914</v>
+      </c>
+      <c r="V35">
+        <f>T35-C35</f>
+        <v>67</v>
+      </c>
+      <c r="W35" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45,88,75,62,88,51,64,52,60,57,81,81,65,63,81,36,55,81,57,60,65,67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>10505</v>
       </c>
@@ -1643,8 +2666,29 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M36" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1,1,1,14,1,1,10,2,1,1,1,1,1,1,1,1,15,2,0,0,0,0,0</v>
+      </c>
+      <c r="N36" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>137</v>
+      </c>
+      <c r="T36" s="5">
+        <v>44913</v>
+      </c>
+      <c r="V36">
+        <f>T36-C36</f>
+        <v>66</v>
+      </c>
+      <c r="W36" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45,88,75,62,88,51,64,52,60,57,81,81,65,63,81,36,55,81,57,60,65,67,66</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>10601</v>
       </c>
@@ -1670,8 +2714,29 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M37" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1,1,1,14,1,1,10,2,1,1,1,1,1,1,1,1,15,2,0,0,0,0,0,3</v>
+      </c>
+      <c r="N37" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>138</v>
+      </c>
+      <c r="T37" s="5">
+        <v>44890</v>
+      </c>
+      <c r="V37">
+        <f>T37-C37</f>
+        <v>42</v>
+      </c>
+      <c r="W37" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45,88,75,62,88,51,64,52,60,57,81,81,65,63,81,36,55,81,57,60,65,67,66,42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>10602</v>
       </c>
@@ -1697,8 +2762,29 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M38" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1,1,1,14,1,1,10,2,1,1,1,1,1,1,1,1,15,2,0,0,0,0,0,3,3</v>
+      </c>
+      <c r="N38" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>100</v>
+      </c>
+      <c r="T38" s="5">
+        <v>44926</v>
+      </c>
+      <c r="V38">
+        <f>T38-C38</f>
+        <v>78</v>
+      </c>
+      <c r="W38" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45,88,75,62,88,51,64,52,60,57,81,81,65,63,81,36,55,81,57,60,65,67,66,42,78</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>10603</v>
       </c>
@@ -1724,8 +2810,29 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M39" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1,1,1,14,1,1,10,2,1,1,1,1,1,1,1,1,15,2,0,0,0,0,0,3,3,3</v>
+      </c>
+      <c r="N39" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>101</v>
+      </c>
+      <c r="T39" s="5">
+        <v>44910</v>
+      </c>
+      <c r="V39">
+        <f>T39-C39</f>
+        <v>62</v>
+      </c>
+      <c r="W39" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45,88,75,62,88,51,64,52,60,57,81,81,65,63,81,36,55,81,57,60,65,67,66,42,78,62</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>10604</v>
       </c>
@@ -1751,8 +2858,29 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M40" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1,1,1,14,1,1,10,2,1,1,1,1,1,1,1,1,15,2,0,0,0,0,0,3,3,3,4</v>
+      </c>
+      <c r="N40" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>102</v>
+      </c>
+      <c r="T40" s="5">
+        <v>44924</v>
+      </c>
+      <c r="V40">
+        <f>T40-C40</f>
+        <v>76</v>
+      </c>
+      <c r="W40" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45,88,75,62,88,51,64,52,60,57,81,81,65,63,81,36,55,81,57,60,65,67,66,42,78,62,76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>10605</v>
       </c>
@@ -1778,8 +2906,29 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M41" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1,1,1,14,1,1,10,2,1,1,1,1,1,1,1,1,15,2,0,0,0,0,0,3,3,3,4,11</v>
+      </c>
+      <c r="N41" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>139</v>
+      </c>
+      <c r="T41" s="5">
+        <v>44887</v>
+      </c>
+      <c r="V41">
+        <f>T41-C41</f>
+        <v>39</v>
+      </c>
+      <c r="W41" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45,88,75,62,88,51,64,52,60,57,81,81,65,63,81,36,55,81,57,60,65,67,66,42,78,62,76,39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>10606</v>
       </c>
@@ -1805,8 +2954,29 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M42" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1,1,1,14,1,1,10,2,1,1,1,1,1,1,1,1,15,2,0,0,0,0,0,3,3,3,4,11,3</v>
+      </c>
+      <c r="N42" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>104</v>
+      </c>
+      <c r="T42" s="5">
+        <v>44863</v>
+      </c>
+      <c r="V42">
+        <f>T42-C42</f>
+        <v>15</v>
+      </c>
+      <c r="W42" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45,88,75,62,88,51,64,52,60,57,81,81,65,63,81,36,55,81,57,60,65,67,66,42,78,62,76,39,15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>10607</v>
       </c>
@@ -1832,8 +3002,29 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M43" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1,1,1,14,1,1,10,2,1,1,1,1,1,1,1,1,15,2,0,0,0,0,0,3,3,3,4,11,3,4</v>
+      </c>
+      <c r="N43" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>140</v>
+      </c>
+      <c r="T43" s="5">
+        <v>44901</v>
+      </c>
+      <c r="V43">
+        <f>T43-C43</f>
+        <v>53</v>
+      </c>
+      <c r="W43" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45,88,75,62,88,51,64,52,60,57,81,81,65,63,81,36,55,81,57,60,65,67,66,42,78,62,76,39,15,53</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>10608</v>
       </c>
@@ -1859,8 +3050,29 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M44" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1,1,1,14,1,1,10,2,1,1,1,1,1,1,1,1,15,2,0,0,0,0,0,3,3,3,4,11,3,4,11</v>
+      </c>
+      <c r="N44" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>141</v>
+      </c>
+      <c r="T44" s="5">
+        <v>44878</v>
+      </c>
+      <c r="V44">
+        <f>T44-C44</f>
+        <v>30</v>
+      </c>
+      <c r="W44" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45,88,75,62,88,51,64,52,60,57,81,81,65,63,81,36,55,81,57,60,65,67,66,42,78,62,76,39,15,53,30</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>10609</v>
       </c>
@@ -1886,8 +3098,29 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M45" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1,1,1,14,1,1,10,2,1,1,1,1,1,1,1,1,15,2,0,0,0,0,0,3,3,3,4,11,3,4,11,4</v>
+      </c>
+      <c r="N45" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>107</v>
+      </c>
+      <c r="T45" s="5">
+        <v>44882</v>
+      </c>
+      <c r="V45">
+        <f>T45-C45</f>
+        <v>34</v>
+      </c>
+      <c r="W45" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45,88,75,62,88,51,64,52,60,57,81,81,65,63,81,36,55,81,57,60,65,67,66,42,78,62,76,39,15,53,30,34</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>10610</v>
       </c>
@@ -1913,8 +3146,29 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M46" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1,1,1,14,1,1,10,2,1,1,1,1,1,1,1,1,15,2,0,0,0,0,0,3,3,3,4,11,3,4,11,4,3</v>
+      </c>
+      <c r="N46" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>142</v>
+      </c>
+      <c r="T46" s="5">
+        <v>44910</v>
+      </c>
+      <c r="V46">
+        <f>T46-C46</f>
+        <v>62</v>
+      </c>
+      <c r="W46" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45,88,75,62,88,51,64,52,60,57,81,81,65,63,81,36,55,81,57,60,65,67,66,42,78,62,76,39,15,53,30,34,62</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>10611</v>
       </c>
@@ -1940,8 +3194,29 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M47" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1,1,1,14,1,1,10,2,1,1,1,1,1,1,1,1,15,2,0,0,0,0,0,3,3,3,4,11,3,4,11,4,3,3</v>
+      </c>
+      <c r="N47" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>109</v>
+      </c>
+      <c r="T47" s="5">
+        <v>44904</v>
+      </c>
+      <c r="V47">
+        <f>T47-C47</f>
+        <v>56</v>
+      </c>
+      <c r="W47" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45,88,75,62,88,51,64,52,60,57,81,81,65,63,81,36,55,81,57,60,65,67,66,42,78,62,76,39,15,53,30,34,62,56</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>10612</v>
       </c>
@@ -1967,8 +3242,29 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M48" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1,1,1,14,1,1,10,2,1,1,1,1,1,1,1,1,15,2,0,0,0,0,0,3,3,3,4,11,3,4,11,4,3,3,3</v>
+      </c>
+      <c r="N48" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>110</v>
+      </c>
+      <c r="T48" s="5">
+        <v>44908</v>
+      </c>
+      <c r="V48">
+        <f>T48-C48</f>
+        <v>60</v>
+      </c>
+      <c r="W48" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45,88,75,62,88,51,64,52,60,57,81,81,65,63,81,36,55,81,57,60,65,67,66,42,78,62,76,39,15,53,30,34,62,56,60</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>10613</v>
       </c>
@@ -1994,8 +3290,29 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M49" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1,1,1,14,1,1,10,2,1,1,1,1,1,1,1,1,15,2,0,0,0,0,0,3,3,3,4,11,3,4,11,4,3,3,3,20</v>
+      </c>
+      <c r="N49" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>111</v>
+      </c>
+      <c r="T49" s="5">
+        <v>44874</v>
+      </c>
+      <c r="V49">
+        <f>T49-C49</f>
+        <v>26</v>
+      </c>
+      <c r="W49" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45,88,75,62,88,51,64,52,60,57,81,81,65,63,81,36,55,81,57,60,65,67,66,42,78,62,76,39,15,53,30,34,62,56,60,26</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>10614</v>
       </c>
@@ -2021,8 +3338,29 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M50" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1,1,1,14,1,1,10,2,1,1,1,1,1,1,1,1,15,2,0,0,0,0,0,3,3,3,4,11,3,4,11,4,3,3,3,20,5</v>
+      </c>
+      <c r="N50" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>143</v>
+      </c>
+      <c r="T50" s="5">
+        <v>44869</v>
+      </c>
+      <c r="V50">
+        <f>T50-C50</f>
+        <v>21</v>
+      </c>
+      <c r="W50" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45,88,75,62,88,51,64,52,60,57,81,81,65,63,81,36,55,81,57,60,65,67,66,42,78,62,76,39,15,53,30,34,62,56,60,26,21</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>10615</v>
       </c>
@@ -2048,8 +3386,29 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M51" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1,1,1,14,1,1,10,2,1,1,1,1,1,1,1,1,15,2,0,0,0,0,0,3,3,3,4,11,3,4,11,4,3,3,3,20,5,0</v>
+      </c>
+      <c r="N51" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>113</v>
+      </c>
+      <c r="T51" s="5">
+        <v>44904</v>
+      </c>
+      <c r="V51">
+        <f>T51-C51</f>
+        <v>51</v>
+      </c>
+      <c r="W51" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45,88,75,62,88,51,64,52,60,57,81,81,65,63,81,36,55,81,57,60,65,67,66,42,78,62,76,39,15,53,30,34,62,56,60,26,21,51</v>
+      </c>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>10616</v>
       </c>
@@ -2075,8 +3434,29 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M52" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1,1,1,14,1,1,10,2,1,1,1,1,1,1,1,1,15,2,0,0,0,0,0,3,3,3,4,11,3,4,11,4,3,3,3,20,5,0,0</v>
+      </c>
+      <c r="N52" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>144</v>
+      </c>
+      <c r="T52" s="5">
+        <v>44889</v>
+      </c>
+      <c r="V52">
+        <f>T52-C52</f>
+        <v>36</v>
+      </c>
+      <c r="W52" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45,88,75,62,88,51,64,52,60,57,81,81,65,63,81,36,55,81,57,60,65,67,66,42,78,62,76,39,15,53,30,34,62,56,60,26,21,51,36</v>
+      </c>
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>10701</v>
       </c>
@@ -2102,8 +3482,29 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M53" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1,1,1,14,1,1,10,2,1,1,1,1,1,1,1,1,15,2,0,0,0,0,0,3,3,3,4,11,3,4,11,4,3,3,3,20,5,0,0,5</v>
+      </c>
+      <c r="N53" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>145</v>
+      </c>
+      <c r="T53" s="5">
+        <v>44919</v>
+      </c>
+      <c r="V53">
+        <f>T53-C53</f>
+        <v>66</v>
+      </c>
+      <c r="W53" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45,88,75,62,88,51,64,52,60,57,81,81,65,63,81,36,55,81,57,60,65,67,66,42,78,62,76,39,15,53,30,34,62,56,60,26,21,51,36,66</v>
+      </c>
+    </row>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>10702</v>
       </c>
@@ -2129,8 +3530,29 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M54" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1,1,1,14,1,1,10,2,1,1,1,1,1,1,1,1,15,2,0,0,0,0,0,3,3,3,4,11,3,4,11,4,3,3,3,20,5,0,0,5,5</v>
+      </c>
+      <c r="N54" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>116</v>
+      </c>
+      <c r="T54" s="5">
+        <v>44915</v>
+      </c>
+      <c r="V54">
+        <f>T54-C54</f>
+        <v>62</v>
+      </c>
+      <c r="W54" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45,88,75,62,88,51,64,52,60,57,81,81,65,63,81,36,55,81,57,60,65,67,66,42,78,62,76,39,15,53,30,34,62,56,60,26,21,51,36,66,62</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>10703</v>
       </c>
@@ -2156,8 +3578,29 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M55" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1,1,1,14,1,1,10,2,1,1,1,1,1,1,1,1,15,2,0,0,0,0,0,3,3,3,4,11,3,4,11,4,3,3,3,20,5,0,0,5,5,2</v>
+      </c>
+      <c r="N55" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>146</v>
+      </c>
+      <c r="T55" s="5">
+        <v>44928</v>
+      </c>
+      <c r="V55">
+        <f>T55-C55</f>
+        <v>75</v>
+      </c>
+      <c r="W55" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45,88,75,62,88,51,64,52,60,57,81,81,65,63,81,36,55,81,57,60,65,67,66,42,78,62,76,39,15,53,30,34,62,56,60,26,21,51,36,66,62,75</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>10704</v>
       </c>
@@ -2183,8 +3626,29 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M56" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1,1,1,14,1,1,10,2,1,1,1,1,1,1,1,1,15,2,0,0,0,0,0,3,3,3,4,11,3,4,11,4,3,3,3,20,5,0,0,5,5,2,9</v>
+      </c>
+      <c r="N56" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>118</v>
+      </c>
+      <c r="T56" s="5">
+        <v>44922</v>
+      </c>
+      <c r="V56">
+        <f>T56-C56</f>
+        <v>69</v>
+      </c>
+      <c r="W56" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45,88,75,62,88,51,64,52,60,57,81,81,65,63,81,36,55,81,57,60,65,67,66,42,78,62,76,39,15,53,30,34,62,56,60,26,21,51,36,66,62,75,69</v>
+      </c>
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>10801</v>
       </c>
@@ -2210,8 +3674,29 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M57" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1,1,1,14,1,1,10,2,1,1,1,1,1,1,1,1,15,2,0,0,0,0,0,3,3,3,4,11,3,4,11,4,3,3,3,20,5,0,0,5,5,2,9,13</v>
+      </c>
+      <c r="N57" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>119</v>
+      </c>
+      <c r="T57" s="5">
+        <v>44943</v>
+      </c>
+      <c r="V57">
+        <f>T57-C57</f>
+        <v>90</v>
+      </c>
+      <c r="W57" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45,88,75,62,88,51,64,52,60,57,81,81,65,63,81,36,55,81,57,60,65,67,66,42,78,62,76,39,15,53,30,34,62,56,60,26,21,51,36,66,62,75,69,90</v>
+      </c>
+    </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>10802</v>
       </c>
@@ -2237,8 +3722,29 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M58" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1,1,1,14,1,1,10,2,1,1,1,1,1,1,1,1,15,2,0,0,0,0,0,3,3,3,4,11,3,4,11,4,3,3,3,20,5,0,0,5,5,2,9,13,13</v>
+      </c>
+      <c r="N58" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>147</v>
+      </c>
+      <c r="T58" s="5">
+        <v>44899</v>
+      </c>
+      <c r="V58">
+        <f>T58-C58</f>
+        <v>46</v>
+      </c>
+      <c r="W58" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45,88,75,62,88,51,64,52,60,57,81,81,65,63,81,36,55,81,57,60,65,67,66,42,78,62,76,39,15,53,30,34,62,56,60,26,21,51,36,66,62,75,69,90,46</v>
+      </c>
+    </row>
+    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>10803</v>
       </c>
@@ -2264,8 +3770,29 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M59" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1,1,1,14,1,1,10,2,1,1,1,1,1,1,1,1,15,2,0,0,0,0,0,3,3,3,4,11,3,4,11,4,3,3,3,20,5,0,0,5,5,2,9,13,13,4</v>
+      </c>
+      <c r="N59" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>121</v>
+      </c>
+      <c r="T59" s="5">
+        <v>44900</v>
+      </c>
+      <c r="V59">
+        <f>T59-C59</f>
+        <v>47</v>
+      </c>
+      <c r="W59" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45,88,75,62,88,51,64,52,60,57,81,81,65,63,81,36,55,81,57,60,65,67,66,42,78,62,76,39,15,53,30,34,62,56,60,26,21,51,36,66,62,75,69,90,46,47</v>
+      </c>
+    </row>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>10804</v>
       </c>
@@ -2291,9 +3818,31 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
+      <c r="M60" t="str">
+        <f t="shared" si="1"/>
+        <v>0,9,5,5,5,5,5,5,5,2,2,23,1,1,1,14,1,1,10,2,1,1,1,1,1,1,1,1,15,2,0,0,0,0,0,3,3,3,4,11,3,4,11,4,3,3,3,20,5,0,0,5,5,2,9,13,13,4,13</v>
+      </c>
+      <c r="N60" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>122</v>
+      </c>
+      <c r="T60" s="5">
+        <v>44907</v>
+      </c>
+      <c r="V60">
+        <f>T60-C60</f>
+        <v>54</v>
+      </c>
+      <c r="W60" t="str">
+        <f t="shared" si="2"/>
+        <v>31,70,82,18,18,68,53,50,71,64,78,39,45,88,75,62,88,51,64,52,60,57,81,81,65,63,81,36,55,81,57,60,65,67,66,42,78,62,76,39,15,53,30,34,62,56,60,26,21,51,36,66,62,75,69,90,46,47,54</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1" xr:uid="{96BA85B1-AB98-4316-911B-E527142C00CD}"/>
+  <autoFilter ref="A1:E1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>